<commit_message>
Documents for Milestone 03 added
</commit_message>
<xml_diff>
--- a/documents/Milestone03/Sprint01UserStories.xlsx
+++ b/documents/Milestone03/Sprint01UserStories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suchiundevia/Documents/grownups/documents/Milestone03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275C9B8A-0864-0C4E-A59E-956AF457054E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B357D97D-9A41-0449-B928-DF39A2816217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28900" yWindow="460" windowWidth="51100" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1249,115 +1249,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">   A user should be able to enter the required information and register an account.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   A user should be informed when the account registration is successful.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   Records should be created when a user creates an account in the relevant tables.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>4.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   If the account creation is unsuccessful, the error message displayed should include site administrator's details for the user.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>5.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   With successful account registration the user should be redirected to the account information page.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>6.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   Any validation on user data that is required should take place before recording in the database.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">   A user should be able to view all the submitted/ recorded account details.
 </t>
     </r>
@@ -1377,115 +1268,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">   A user should be able to view any files they have uploaded, including images.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   A user should be able to delete their account.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>2.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   The database should remove the registered user's details.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   A confirmation prompt should appear for the user to confirm deletion.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>4.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   A confirmation message is required to be displayed or the user.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>5.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   If an error occurs, the site administrators  details should be displayed to the user for troubleshooting.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>6.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">   A user must have an account in order to delete it.</t>
     </r>
   </si>
   <si>
@@ -2321,12 +2103,230 @@
     <t>1.   Facebook account connection should be seen under user profile.
 2.   These connections should be optional.</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   A user should be able to enter the required information and register an account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   A user should be informed when the account registration is successful.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   Records should be created when a user creates an account in the relevant tables.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   If the account creation is unsuccessful, the error message displayed should include site administrator's details for the user.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   With successful account registration the user should be redirected to the login page.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>6.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   Any validation on user data that is required should take place before recording in the database.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   A user should be able to delete their account.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   The database should remove the registered user's details and any other entries.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   A confirmation prompt should appear for the user to confirm deletion.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   A confirmation message is required to be displayed or the user.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   If an error occurs, the site administrators  details should be displayed to the user for troubleshooting.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>6.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   A user must have an account in order to delete it.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2461,8 +2461,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2519,25 +2525,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC0CBF3"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE9C5F4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2868,49 +2868,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2948,6 +2906,48 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3282,8 +3282,8 @@
   </sheetPr>
   <dimension ref="A1:AB1036"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3300,18 +3300,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="33.75" customHeight="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -3382,35 +3382,35 @@
       <c r="AB2" s="5"/>
     </row>
     <row r="3" spans="1:28" ht="57">
-      <c r="A3" s="54">
+      <c r="A3" s="79">
         <v>1</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="F3" s="59">
+      <c r="F3" s="76">
         <v>10</v>
       </c>
       <c r="G3" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="55" t="s">
+      <c r="I3" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="60" t="s">
-        <v>249</v>
+      <c r="J3" s="78" t="s">
+        <v>247</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -3432,34 +3432,34 @@
       <c r="AB3" s="1"/>
     </row>
     <row r="4" spans="1:28" ht="57">
-      <c r="A4" s="54">
+      <c r="A4" s="79">
         <v>2</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="59">
+      <c r="F4" s="76">
         <v>4</v>
       </c>
       <c r="G4" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="55" t="s">
+      <c r="I4" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="78" t="s">
         <v>35</v>
       </c>
       <c r="K4" s="1"/>
@@ -3482,34 +3482,34 @@
       <c r="AB4" s="1"/>
     </row>
     <row r="5" spans="1:28" ht="95">
-      <c r="A5" s="54">
+      <c r="A5" s="79">
         <v>3</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="F5" s="59">
+      <c r="F5" s="76">
         <v>20</v>
       </c>
       <c r="G5" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="59" t="s">
+      <c r="H5" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="78" t="s">
         <v>39</v>
       </c>
       <c r="K5" s="1"/>
@@ -3532,34 +3532,34 @@
       <c r="AB5" s="1"/>
     </row>
     <row r="6" spans="1:28" ht="38">
-      <c r="A6" s="54">
+      <c r="A6" s="79">
         <v>4</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="F6" s="59">
+      <c r="F6" s="76">
         <v>2</v>
       </c>
       <c r="G6" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="55" t="s">
+      <c r="I6" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="78" t="s">
         <v>44</v>
       </c>
       <c r="K6" s="1"/>
@@ -3582,34 +3582,34 @@
       <c r="AB6" s="1"/>
     </row>
     <row r="7" spans="1:28" ht="38">
-      <c r="A7" s="54">
+      <c r="A7" s="79">
         <v>5</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="77" t="s">
         <v>129</v>
       </c>
-      <c r="F7" s="59">
+      <c r="F7" s="76">
         <v>2</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H7" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="55" t="s">
+      <c r="I7" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="60" t="s">
+      <c r="J7" s="78" t="s">
         <v>48</v>
       </c>
       <c r="K7" s="1"/>
@@ -3632,34 +3632,34 @@
       <c r="AB7" s="1"/>
     </row>
     <row r="8" spans="1:28" ht="38">
-      <c r="A8" s="54">
+      <c r="A8" s="79">
         <v>6</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="F8" s="59">
+      <c r="F8" s="76">
         <v>6</v>
       </c>
       <c r="G8" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="78" t="s">
         <v>51</v>
       </c>
       <c r="K8" s="1"/>
@@ -4082,34 +4082,34 @@
       <c r="AB16" s="1"/>
     </row>
     <row r="17" spans="1:28" ht="128" customHeight="1">
-      <c r="A17" s="52">
+      <c r="A17" s="69">
         <v>15</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="53" t="s">
+      <c r="D17" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="53" t="s">
-        <v>139</v>
+      <c r="E17" s="82" t="s">
+        <v>249</v>
       </c>
-      <c r="F17" s="64">
+      <c r="F17" s="70">
         <v>20</v>
       </c>
       <c r="G17" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="64" t="s">
+      <c r="H17" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="53" t="s">
+      <c r="I17" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="J17" s="65" t="s">
+      <c r="J17" s="71" t="s">
         <v>79</v>
       </c>
       <c r="K17" s="1"/>
@@ -4132,34 +4132,34 @@
       <c r="AB17" s="1"/>
     </row>
     <row r="18" spans="1:28" ht="38">
-      <c r="A18" s="52">
+      <c r="A18" s="69">
         <v>16</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="53" t="s">
+      <c r="C18" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="53" t="s">
-        <v>140</v>
+      <c r="E18" s="52" t="s">
+        <v>139</v>
       </c>
-      <c r="F18" s="64">
+      <c r="F18" s="70">
         <v>9</v>
       </c>
       <c r="G18" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="64" t="s">
+      <c r="H18" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I18" s="53" t="s">
+      <c r="I18" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="65" t="s">
+      <c r="J18" s="71" t="s">
         <v>83</v>
       </c>
       <c r="K18" s="1"/>
@@ -4182,34 +4182,34 @@
       <c r="AB18" s="1"/>
     </row>
     <row r="19" spans="1:28" ht="114">
-      <c r="A19" s="52">
+      <c r="A19" s="69">
         <v>17</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="53" t="s">
+      <c r="D19" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="53" t="s">
-        <v>141</v>
+      <c r="E19" s="82" t="s">
+        <v>250</v>
       </c>
-      <c r="F19" s="64">
+      <c r="F19" s="70">
         <v>7</v>
       </c>
       <c r="G19" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="64" t="s">
+      <c r="H19" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="53" t="s">
+      <c r="I19" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="J19" s="65" t="s">
+      <c r="J19" s="71" t="s">
         <v>86</v>
       </c>
       <c r="K19" s="1"/>
@@ -4232,34 +4232,34 @@
       <c r="AB19" s="1"/>
     </row>
     <row r="20" spans="1:28" ht="95">
-      <c r="A20" s="52">
+      <c r="A20" s="69">
         <v>18</v>
       </c>
-      <c r="B20" s="53" t="s">
+      <c r="B20" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="53" t="s">
-        <v>142</v>
+      <c r="E20" s="52" t="s">
+        <v>140</v>
       </c>
-      <c r="F20" s="64">
+      <c r="F20" s="70">
         <v>5</v>
       </c>
       <c r="G20" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="64" t="s">
+      <c r="H20" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="53" t="s">
+      <c r="I20" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="65" t="s">
+      <c r="J20" s="71" t="s">
         <v>89</v>
       </c>
       <c r="K20" s="1"/>
@@ -4282,34 +4282,34 @@
       <c r="AB20" s="1"/>
     </row>
     <row r="21" spans="1:28" ht="57">
-      <c r="A21" s="52">
+      <c r="A21" s="69">
         <v>19</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="53" t="s">
-        <v>143</v>
+      <c r="E21" s="52" t="s">
+        <v>141</v>
       </c>
-      <c r="F21" s="64">
+      <c r="F21" s="70">
         <v>2</v>
       </c>
       <c r="G21" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="64" t="s">
+      <c r="H21" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="53" t="s">
+      <c r="I21" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="65" t="s">
+      <c r="J21" s="71" t="s">
         <v>92</v>
       </c>
       <c r="K21" s="1"/>
@@ -4332,34 +4332,34 @@
       <c r="AB21" s="1"/>
     </row>
     <row r="22" spans="1:28" ht="95">
-      <c r="A22" s="52">
+      <c r="A22" s="69">
         <v>20</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="53" t="s">
+      <c r="D22" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="53" t="s">
-        <v>144</v>
+      <c r="E22" s="52" t="s">
+        <v>142</v>
       </c>
-      <c r="F22" s="64">
+      <c r="F22" s="70">
         <v>2</v>
       </c>
       <c r="G22" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="64" t="s">
+      <c r="H22" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="53" t="s">
+      <c r="I22" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="65" t="s">
+      <c r="J22" s="71" t="s">
         <v>95</v>
       </c>
       <c r="K22" s="1"/>
@@ -4382,34 +4382,34 @@
       <c r="AB22" s="1"/>
     </row>
     <row r="23" spans="1:28" ht="76" hidden="1">
-      <c r="A23" s="52">
+      <c r="A23" s="69">
         <v>21</v>
       </c>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="53" t="s">
+      <c r="D23" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="53" t="s">
-        <v>145</v>
+      <c r="E23" s="52" t="s">
+        <v>143</v>
       </c>
-      <c r="F23" s="64">
+      <c r="F23" s="70">
         <v>4</v>
       </c>
       <c r="G23" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="64" t="s">
+      <c r="H23" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="53" t="s">
+      <c r="I23" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="65" t="s">
+      <c r="J23" s="71" t="s">
         <v>98</v>
       </c>
       <c r="K23" s="1"/>
@@ -4432,34 +4432,34 @@
       <c r="AB23" s="1"/>
     </row>
     <row r="24" spans="1:28" ht="38" hidden="1">
-      <c r="A24" s="52">
+      <c r="A24" s="69">
         <v>22</v>
       </c>
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="53" t="s">
+      <c r="C24" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="53" t="s">
+      <c r="D24" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="53" t="s">
-        <v>146</v>
+      <c r="E24" s="52" t="s">
+        <v>144</v>
       </c>
-      <c r="F24" s="64">
+      <c r="F24" s="70">
         <v>3</v>
       </c>
       <c r="G24" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H24" s="64" t="s">
+      <c r="H24" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I24" s="53" t="s">
+      <c r="I24" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="J24" s="65" t="s">
+      <c r="J24" s="71" t="s">
         <v>102</v>
       </c>
       <c r="K24" s="1"/>
@@ -4482,34 +4482,34 @@
       <c r="AB24" s="1"/>
     </row>
     <row r="25" spans="1:28" ht="57" hidden="1">
-      <c r="A25" s="52">
+      <c r="A25" s="69">
         <v>23</v>
       </c>
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D25" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="53" t="s">
-        <v>147</v>
+      <c r="E25" s="52" t="s">
+        <v>145</v>
       </c>
-      <c r="F25" s="64">
+      <c r="F25" s="70">
         <v>3</v>
       </c>
       <c r="G25" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="64" t="s">
+      <c r="H25" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="53" t="s">
+      <c r="I25" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="J25" s="65" t="s">
+      <c r="J25" s="71" t="s">
         <v>105</v>
       </c>
       <c r="K25" s="1"/>
@@ -4532,34 +4532,34 @@
       <c r="AB25" s="1"/>
     </row>
     <row r="26" spans="1:28" ht="57">
-      <c r="A26" s="52">
+      <c r="A26" s="69">
         <v>24</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="53" t="s">
+      <c r="C26" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="53" t="s">
+      <c r="D26" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="53" t="s">
-        <v>148</v>
+      <c r="E26" s="52" t="s">
+        <v>146</v>
       </c>
-      <c r="F26" s="64">
+      <c r="F26" s="70">
         <v>20</v>
       </c>
       <c r="G26" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="64" t="s">
+      <c r="H26" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="53" t="s">
+      <c r="I26" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="J26" s="65" t="s">
+      <c r="J26" s="71" t="s">
         <v>108</v>
       </c>
       <c r="K26" s="1"/>
@@ -4582,34 +4582,34 @@
       <c r="AB26" s="1"/>
     </row>
     <row r="27" spans="1:28" ht="57">
-      <c r="A27" s="57">
+      <c r="A27" s="75">
         <v>25</v>
       </c>
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="58" t="s">
+      <c r="C27" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="58" t="s">
+      <c r="D27" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="58" t="s">
-        <v>149</v>
+      <c r="E27" s="73" t="s">
+        <v>147</v>
       </c>
-      <c r="F27" s="61">
+      <c r="F27" s="72">
         <v>10</v>
       </c>
       <c r="G27" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="61" t="s">
+      <c r="H27" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I27" s="58" t="s">
+      <c r="I27" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="J27" s="62" t="s">
+      <c r="J27" s="74" t="s">
         <v>111</v>
       </c>
       <c r="K27" s="1"/>
@@ -4632,34 +4632,34 @@
       <c r="AB27" s="1"/>
     </row>
     <row r="28" spans="1:28" ht="57">
-      <c r="A28" s="57">
+      <c r="A28" s="75">
         <v>26</v>
       </c>
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D28" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="E28" s="58" t="s">
+      <c r="E28" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="61">
+      <c r="F28" s="72">
         <v>4</v>
       </c>
       <c r="G28" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="61" t="s">
+      <c r="H28" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="58" t="s">
+      <c r="I28" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="J28" s="62" t="s">
+      <c r="J28" s="74" t="s">
         <v>122</v>
       </c>
       <c r="K28" s="2"/>
@@ -4682,35 +4682,35 @@
       <c r="AB28" s="2"/>
     </row>
     <row r="29" spans="1:28" ht="57" hidden="1">
-      <c r="A29" s="57">
+      <c r="A29" s="75">
         <v>27</v>
       </c>
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="58" t="s">
+      <c r="C29" s="73" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="58" t="s">
-        <v>239</v>
+      <c r="D29" s="73" t="s">
+        <v>237</v>
       </c>
-      <c r="E29" s="58" t="s">
+      <c r="E29" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="F29" s="61">
+      <c r="F29" s="72">
         <v>3</v>
       </c>
       <c r="G29" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="61" t="s">
+      <c r="H29" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I29" s="58" t="s">
+      <c r="I29" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="62" t="s">
-        <v>150</v>
+      <c r="J29" s="74" t="s">
+        <v>148</v>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -4732,35 +4732,35 @@
       <c r="AB29" s="2"/>
     </row>
     <row r="30" spans="1:28" ht="38">
-      <c r="A30" s="57">
+      <c r="A30" s="75">
         <v>28</v>
       </c>
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="73" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" s="73" t="s">
         <v>151</v>
       </c>
-      <c r="C30" s="58" t="s">
-        <v>152</v>
-      </c>
-      <c r="D30" s="58" t="s">
+      <c r="E30" s="73" t="s">
         <v>153</v>
       </c>
-      <c r="E30" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="F30" s="61">
+      <c r="F30" s="72">
         <v>6</v>
       </c>
       <c r="G30" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="H30" s="61" t="s">
+      <c r="H30" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="58" t="s">
+      <c r="I30" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="J30" s="62" t="s">
-        <v>154</v>
+      <c r="J30" s="74" t="s">
+        <v>152</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -4782,35 +4782,35 @@
       <c r="AB30" s="2"/>
     </row>
     <row r="31" spans="1:28" ht="38">
-      <c r="A31" s="57">
+      <c r="A31" s="75">
         <v>29</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="58" t="s">
-        <v>156</v>
+      <c r="C31" s="73" t="s">
+        <v>154</v>
       </c>
-      <c r="D31" s="58" t="s">
-        <v>157</v>
+      <c r="D31" s="73" t="s">
+        <v>155</v>
       </c>
-      <c r="E31" s="58" t="s">
-        <v>250</v>
+      <c r="E31" s="73" t="s">
+        <v>248</v>
       </c>
-      <c r="F31" s="61">
+      <c r="F31" s="72">
         <v>20</v>
       </c>
       <c r="G31" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H31" s="61" t="s">
+      <c r="H31" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I31" s="58" t="s">
+      <c r="I31" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="J31" s="63" t="s">
-        <v>159</v>
+      <c r="J31" s="81" t="s">
+        <v>157</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -4832,35 +4832,35 @@
       <c r="AB31" s="2"/>
     </row>
     <row r="32" spans="1:28" ht="38" hidden="1">
-      <c r="A32" s="57">
+      <c r="A32" s="75">
         <v>30</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="58" t="s">
-        <v>160</v>
+      <c r="C32" s="73" t="s">
+        <v>158</v>
       </c>
-      <c r="D32" s="58" t="s">
-        <v>161</v>
+      <c r="D32" s="73" t="s">
+        <v>159</v>
       </c>
-      <c r="E32" s="58" t="s">
-        <v>166</v>
+      <c r="E32" s="73" t="s">
+        <v>164</v>
       </c>
-      <c r="F32" s="61">
+      <c r="F32" s="72">
         <v>4</v>
       </c>
       <c r="G32" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H32" s="61" t="s">
+      <c r="H32" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="58" t="s">
+      <c r="I32" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="J32" s="62" t="s">
-        <v>162</v>
+      <c r="J32" s="74" t="s">
+        <v>160</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -4882,35 +4882,35 @@
       <c r="AB32" s="2"/>
     </row>
     <row r="33" spans="1:28" ht="76" hidden="1">
-      <c r="A33" s="57">
+      <c r="A33" s="75">
         <v>31</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="58" t="s">
+      <c r="C33" s="73" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="73" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="D33" s="58" t="s">
-        <v>164</v>
-      </c>
-      <c r="E33" s="58" t="s">
-        <v>165</v>
-      </c>
-      <c r="F33" s="61">
+      <c r="F33" s="72">
         <v>6</v>
       </c>
       <c r="G33" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H33" s="61" t="s">
+      <c r="H33" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I33" s="58" t="s">
+      <c r="I33" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="62" t="s">
-        <v>240</v>
+      <c r="J33" s="74" t="s">
+        <v>238</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -4932,35 +4932,35 @@
       <c r="AB33" s="2"/>
     </row>
     <row r="34" spans="1:28" ht="76" hidden="1">
-      <c r="A34" s="57">
+      <c r="A34" s="75">
         <v>32</v>
       </c>
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="58" t="s">
+      <c r="C34" s="73" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="73" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" s="73" t="s">
         <v>167</v>
       </c>
-      <c r="D34" s="58" t="s">
-        <v>168</v>
-      </c>
-      <c r="E34" s="58" t="s">
-        <v>169</v>
-      </c>
-      <c r="F34" s="61">
+      <c r="F34" s="72">
         <v>5</v>
       </c>
       <c r="G34" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H34" s="61" t="s">
+      <c r="H34" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="58" t="s">
+      <c r="I34" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="J34" s="62" t="s">
-        <v>240</v>
+      <c r="J34" s="74" t="s">
+        <v>238</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -4982,35 +4982,35 @@
       <c r="AB34" s="2"/>
     </row>
     <row r="35" spans="1:28" ht="57" hidden="1">
-      <c r="A35" s="57">
+      <c r="A35" s="75">
         <v>33</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="58" t="s">
+      <c r="C35" s="73" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" s="73" t="s">
+        <v>169</v>
+      </c>
+      <c r="E35" s="73" t="s">
         <v>170</v>
       </c>
-      <c r="D35" s="58" t="s">
-        <v>171</v>
-      </c>
-      <c r="E35" s="58" t="s">
-        <v>172</v>
-      </c>
-      <c r="F35" s="61">
+      <c r="F35" s="72">
         <v>6</v>
       </c>
       <c r="G35" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H35" s="61" t="s">
+      <c r="H35" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I35" s="58" t="s">
+      <c r="I35" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="J35" s="62" t="s">
-        <v>173</v>
+      <c r="J35" s="74" t="s">
+        <v>171</v>
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -5032,35 +5032,35 @@
       <c r="AB35" s="2"/>
     </row>
     <row r="36" spans="1:28" ht="57" hidden="1">
-      <c r="A36" s="57">
+      <c r="A36" s="75">
         <v>34</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="58" t="s">
+      <c r="C36" s="73" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" s="73" t="s">
+        <v>173</v>
+      </c>
+      <c r="E36" s="73" t="s">
         <v>174</v>
       </c>
-      <c r="D36" s="58" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" s="58" t="s">
-        <v>176</v>
-      </c>
-      <c r="F36" s="61">
+      <c r="F36" s="72">
         <v>10</v>
       </c>
       <c r="G36" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H36" s="61" t="s">
+      <c r="H36" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="58" t="s">
+      <c r="I36" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="J36" s="62" t="s">
-        <v>241</v>
+      <c r="J36" s="74" t="s">
+        <v>239</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -5082,35 +5082,35 @@
       <c r="AB36" s="2"/>
     </row>
     <row r="37" spans="1:28" ht="76" hidden="1">
-      <c r="A37" s="57">
+      <c r="A37" s="75">
         <v>35</v>
       </c>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="58" t="s">
+      <c r="C37" s="73" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="73" t="s">
+        <v>176</v>
+      </c>
+      <c r="E37" s="73" t="s">
         <v>177</v>
       </c>
-      <c r="D37" s="58" t="s">
-        <v>178</v>
-      </c>
-      <c r="E37" s="58" t="s">
-        <v>179</v>
-      </c>
-      <c r="F37" s="61">
+      <c r="F37" s="72">
         <v>20</v>
       </c>
       <c r="G37" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H37" s="61" t="s">
+      <c r="H37" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="58" t="s">
+      <c r="I37" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="62" t="s">
-        <v>180</v>
+      <c r="J37" s="74" t="s">
+        <v>178</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -5132,35 +5132,35 @@
       <c r="AB37" s="2"/>
     </row>
     <row r="38" spans="1:28" ht="76" hidden="1">
-      <c r="A38" s="57">
+      <c r="A38" s="75">
         <v>36</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="B38" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="58" t="s">
-        <v>181</v>
+      <c r="C38" s="73" t="s">
+        <v>179</v>
       </c>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="73" t="s">
+        <v>180</v>
+      </c>
+      <c r="E38" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="E38" s="58" t="s">
-        <v>184</v>
-      </c>
-      <c r="F38" s="61">
+      <c r="F38" s="72">
         <v>10</v>
       </c>
       <c r="G38" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H38" s="61" t="s">
+      <c r="H38" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="58" t="s">
+      <c r="I38" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="J38" s="62" t="s">
-        <v>183</v>
+      <c r="J38" s="74" t="s">
+        <v>181</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -5182,35 +5182,35 @@
       <c r="AB38" s="2"/>
     </row>
     <row r="39" spans="1:28" ht="76" hidden="1">
-      <c r="A39" s="57">
+      <c r="A39" s="75">
         <v>37</v>
       </c>
-      <c r="B39" s="58" t="s">
-        <v>151</v>
+      <c r="B39" s="73" t="s">
+        <v>149</v>
       </c>
-      <c r="C39" s="58" t="s">
+      <c r="C39" s="73" t="s">
+        <v>183</v>
+      </c>
+      <c r="D39" s="73" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" s="73" t="s">
         <v>185</v>
       </c>
-      <c r="D39" s="58" t="s">
-        <v>186</v>
-      </c>
-      <c r="E39" s="58" t="s">
-        <v>187</v>
-      </c>
-      <c r="F39" s="61">
+      <c r="F39" s="72">
         <v>3</v>
       </c>
       <c r="G39" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H39" s="61" t="s">
+      <c r="H39" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I39" s="58" t="s">
+      <c r="I39" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="J39" s="62" t="s">
-        <v>188</v>
+      <c r="J39" s="74" t="s">
+        <v>186</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -5232,35 +5232,35 @@
       <c r="AB39" s="2"/>
     </row>
     <row r="40" spans="1:28" ht="57">
-      <c r="A40" s="57">
+      <c r="A40" s="75">
         <v>38</v>
       </c>
-      <c r="B40" s="58" t="s">
+      <c r="B40" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="58" t="s">
-        <v>242</v>
+      <c r="C40" s="73" t="s">
+        <v>240</v>
       </c>
-      <c r="D40" s="58" t="s">
-        <v>189</v>
+      <c r="D40" s="73" t="s">
+        <v>187</v>
       </c>
-      <c r="E40" s="58" t="s">
-        <v>243</v>
+      <c r="E40" s="73" t="s">
+        <v>241</v>
       </c>
-      <c r="F40" s="61">
+      <c r="F40" s="72">
         <v>10</v>
       </c>
       <c r="G40" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H40" s="61" t="s">
+      <c r="H40" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I40" s="58" t="s">
+      <c r="I40" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="J40" s="62" t="s">
-        <v>190</v>
+      <c r="J40" s="74" t="s">
+        <v>188</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -5282,35 +5282,35 @@
       <c r="AB40" s="2"/>
     </row>
     <row r="41" spans="1:28" ht="38" hidden="1">
-      <c r="A41" s="57">
+      <c r="A41" s="75">
         <v>39</v>
       </c>
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="58" t="s">
-        <v>191</v>
+      <c r="C41" s="73" t="s">
+        <v>189</v>
       </c>
-      <c r="D41" s="58" t="s">
-        <v>192</v>
+      <c r="D41" s="73" t="s">
+        <v>190</v>
       </c>
-      <c r="E41" s="58" t="s">
-        <v>244</v>
+      <c r="E41" s="73" t="s">
+        <v>242</v>
       </c>
-      <c r="F41" s="61">
+      <c r="F41" s="72">
         <v>8</v>
       </c>
       <c r="G41" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H41" s="61" t="s">
+      <c r="H41" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I41" s="58" t="s">
+      <c r="I41" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="J41" s="62" t="s">
-        <v>193</v>
+      <c r="J41" s="74" t="s">
+        <v>191</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -5332,35 +5332,35 @@
       <c r="AB41" s="2"/>
     </row>
     <row r="42" spans="1:28" ht="38" hidden="1">
-      <c r="A42" s="57">
+      <c r="A42" s="75">
         <v>40</v>
       </c>
-      <c r="B42" s="58" t="s">
+      <c r="B42" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="58" t="s">
+      <c r="C42" s="73" t="s">
+        <v>192</v>
+      </c>
+      <c r="D42" s="73" t="s">
+        <v>193</v>
+      </c>
+      <c r="E42" s="73" t="s">
         <v>194</v>
       </c>
-      <c r="D42" s="58" t="s">
-        <v>195</v>
-      </c>
-      <c r="E42" s="58" t="s">
-        <v>196</v>
-      </c>
-      <c r="F42" s="61">
+      <c r="F42" s="72">
         <v>5</v>
       </c>
       <c r="G42" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H42" s="61" t="s">
+      <c r="H42" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I42" s="58" t="s">
+      <c r="I42" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="J42" s="62" t="s">
-        <v>197</v>
+      <c r="J42" s="74" t="s">
+        <v>195</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -5382,35 +5382,35 @@
       <c r="AB42" s="2"/>
     </row>
     <row r="43" spans="1:28" ht="38" hidden="1">
-      <c r="A43" s="57">
+      <c r="A43" s="75">
         <v>41</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="73" t="s">
+        <v>196</v>
+      </c>
+      <c r="D43" s="73" t="s">
+        <v>193</v>
+      </c>
+      <c r="E43" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="D43" s="58" t="s">
-        <v>195</v>
-      </c>
-      <c r="E43" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="F43" s="61">
+      <c r="F43" s="72">
         <v>5</v>
       </c>
       <c r="G43" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H43" s="61" t="s">
+      <c r="H43" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I43" s="58" t="s">
+      <c r="I43" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="J43" s="62" t="s">
-        <v>199</v>
+      <c r="J43" s="74" t="s">
+        <v>197</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -5432,35 +5432,35 @@
       <c r="AB43" s="2"/>
     </row>
     <row r="44" spans="1:28" ht="38" hidden="1">
-      <c r="A44" s="57">
+      <c r="A44" s="75">
         <v>42</v>
       </c>
-      <c r="B44" s="58" t="s">
+      <c r="B44" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="58" t="s">
+      <c r="C44" s="73" t="s">
+        <v>199</v>
+      </c>
+      <c r="D44" s="73" t="s">
+        <v>200</v>
+      </c>
+      <c r="E44" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="D44" s="58" t="s">
-        <v>202</v>
-      </c>
-      <c r="E44" s="58" t="s">
-        <v>203</v>
-      </c>
-      <c r="F44" s="61">
+      <c r="F44" s="72">
         <v>4</v>
       </c>
       <c r="G44" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H44" s="61" t="s">
+      <c r="H44" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I44" s="58" t="s">
+      <c r="I44" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="J44" s="62" t="s">
-        <v>204</v>
+      <c r="J44" s="74" t="s">
+        <v>202</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -5482,35 +5482,35 @@
       <c r="AB44" s="2"/>
     </row>
     <row r="45" spans="1:28" ht="57" hidden="1">
-      <c r="A45" s="57">
+      <c r="A45" s="75">
         <v>43</v>
       </c>
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="58" t="s">
+      <c r="C45" s="73" t="s">
+        <v>203</v>
+      </c>
+      <c r="D45" s="73" t="s">
+        <v>204</v>
+      </c>
+      <c r="E45" s="73" t="s">
         <v>205</v>
       </c>
-      <c r="D45" s="58" t="s">
-        <v>206</v>
-      </c>
-      <c r="E45" s="58" t="s">
-        <v>207</v>
-      </c>
-      <c r="F45" s="61">
+      <c r="F45" s="72">
         <v>4</v>
       </c>
       <c r="G45" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H45" s="61" t="s">
+      <c r="H45" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I45" s="58" t="s">
+      <c r="I45" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="J45" s="62" t="s">
-        <v>208</v>
+      <c r="J45" s="74" t="s">
+        <v>206</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
@@ -5532,35 +5532,35 @@
       <c r="AB45" s="2"/>
     </row>
     <row r="46" spans="1:28" ht="57">
-      <c r="A46" s="57">
+      <c r="A46" s="75">
         <v>44</v>
       </c>
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C46" s="58" t="s">
-        <v>209</v>
+      <c r="C46" s="73" t="s">
+        <v>207</v>
       </c>
-      <c r="D46" s="58" t="s">
-        <v>210</v>
+      <c r="D46" s="73" t="s">
+        <v>208</v>
       </c>
-      <c r="E46" s="58" t="s">
-        <v>245</v>
+      <c r="E46" s="73" t="s">
+        <v>243</v>
       </c>
-      <c r="F46" s="61">
+      <c r="F46" s="72">
         <v>3</v>
       </c>
       <c r="G46" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="H46" s="61" t="s">
+      <c r="H46" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I46" s="58" t="s">
+      <c r="I46" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="J46" s="62" t="s">
-        <v>211</v>
+      <c r="J46" s="74" t="s">
+        <v>209</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -5586,16 +5586,16 @@
         <v>45</v>
       </c>
       <c r="B47" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D47" s="34" t="s">
         <v>94</v>
       </c>
       <c r="E47" s="34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F47" s="35">
         <v>3</v>
@@ -5604,13 +5604,13 @@
         <v>42</v>
       </c>
       <c r="H47" s="44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I47" s="34" t="s">
         <v>4</v>
       </c>
       <c r="J47" s="37" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
@@ -5639,13 +5639,13 @@
         <v>80</v>
       </c>
       <c r="C48" s="34" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E48" s="34" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F48" s="42">
         <v>5</v>
@@ -5654,13 +5654,13 @@
         <v>42</v>
       </c>
       <c r="H48" s="44" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I48" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J48" s="37" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
@@ -5689,13 +5689,13 @@
         <v>80</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D49" s="34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E49" s="34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F49" s="35">
         <v>10</v>
@@ -5704,13 +5704,13 @@
         <v>42</v>
       </c>
       <c r="H49" s="44" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I49" s="34" t="s">
         <v>5</v>
       </c>
       <c r="J49" s="37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
@@ -5739,13 +5739,13 @@
         <v>73</v>
       </c>
       <c r="C50" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E50" s="34" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F50" s="35">
         <v>2</v>
@@ -5754,13 +5754,13 @@
         <v>42</v>
       </c>
       <c r="H50" s="44" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I50" s="34" t="s">
         <v>5</v>
       </c>
       <c r="J50" s="37" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
@@ -5789,13 +5789,13 @@
         <v>73</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D51" s="34" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E51" s="34" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F51" s="35">
         <v>3</v>
@@ -5804,13 +5804,13 @@
         <v>42</v>
       </c>
       <c r="H51" s="44" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I51" s="34" t="s">
         <v>5</v>
       </c>
       <c r="J51" s="37" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -5839,13 +5839,13 @@
         <v>36</v>
       </c>
       <c r="C52" s="34" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D52" s="34" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E52" s="34" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F52" s="35">
         <v>2</v>
@@ -5854,13 +5854,13 @@
         <v>42</v>
       </c>
       <c r="H52" s="44" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I52" s="34" t="s">
         <v>4</v>
       </c>
       <c r="J52" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
@@ -5889,13 +5889,13 @@
         <v>73</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E53" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F53" s="35">
         <v>2</v>
@@ -5904,13 +5904,13 @@
         <v>42</v>
       </c>
       <c r="H53" s="44" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I53" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J53" s="37" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
@@ -35459,17 +35459,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="31" customHeight="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
       <c r="L1" s="20"/>
@@ -35490,15 +35490,15 @@
       <c r="AA1" s="20"/>
     </row>
     <row r="2" spans="1:27" ht="18">
-      <c r="A2" s="74"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="76"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
       <c r="L2" s="20"/>
@@ -35744,13 +35744,13 @@
       <c r="B10" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
       <c r="J10" s="20"/>
@@ -35775,11 +35775,11 @@
     <row r="11" spans="1:27" ht="18">
       <c r="A11" s="27"/>
       <c r="B11" s="29"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
       <c r="J11" s="20"/>
@@ -35806,13 +35806,13 @@
       <c r="B12" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
       <c r="J12" s="20"/>
@@ -35837,11 +35837,11 @@
     <row r="13" spans="1:27" ht="18">
       <c r="A13" s="27"/>
       <c r="B13" s="29"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="20"/>
@@ -35868,13 +35868,13 @@
       <c r="B14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="78" t="s">
+      <c r="C14" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="20"/>
@@ -35899,11 +35899,11 @@
     <row r="15" spans="1:27" ht="18">
       <c r="A15" s="27"/>
       <c r="B15" s="29"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
       <c r="J15" s="20"/>
@@ -35930,13 +35930,13 @@
       <c r="B16" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="70" t="s">
+      <c r="C16" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
       <c r="J16" s="20"/>
@@ -35961,11 +35961,11 @@
     <row r="17" spans="1:27" ht="18">
       <c r="A17" s="27"/>
       <c r="B17" s="29"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
       <c r="J17" s="20"/>
@@ -35992,13 +35992,13 @@
       <c r="B18" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="70" t="s">
+      <c r="C18" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
       <c r="H18" s="28"/>
       <c r="I18" s="28"/>
       <c r="J18" s="20"/>
@@ -64787,52 +64787,52 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:20" ht="30" customHeight="1">
-      <c r="A1" s="79" t="s">
-        <v>248</v>
+      <c r="A1" s="65" t="s">
+        <v>246</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
     </row>
     <row r="2" spans="1:20" ht="30" customHeight="1">
-      <c r="A2" s="81" t="s">
-        <v>247</v>
+      <c r="A2" s="67" t="s">
+        <v>245</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="82"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>